<commit_message>
Add userlist in GetUser method because the user list was created 3 times (each call)
</commit_message>
<xml_diff>
--- a/Users/Users-IUCT.xlsx
+++ b/Users/Users-IUCT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="148">
   <si>
     <t>Id</t>
   </si>
@@ -355,6 +355,114 @@
   </si>
   <si>
     <t>Mickael</t>
+  </si>
+  <si>
+    <t>Bisque</t>
+  </si>
+  <si>
+    <t>Indigo</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Coral</t>
+  </si>
+  <si>
+    <t>DarkGreen</t>
+  </si>
+  <si>
+    <t>Chartreuse</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>HotPink</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>CornflowerBlue</t>
+  </si>
+  <si>
+    <t>AntiqueWhite</t>
+  </si>
+  <si>
+    <t>Aquamarine</t>
+  </si>
+  <si>
+    <t>GreenYellow</t>
+  </si>
+  <si>
+    <t>YellowGreen</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>MediumTurquoise</t>
+  </si>
+  <si>
+    <t>PaleVioletRed</t>
+  </si>
+  <si>
+    <t>LightSalmon</t>
+  </si>
+  <si>
+    <t>Tan</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>DeepPink</t>
+  </si>
+  <si>
+    <t>Khaki</t>
+  </si>
+  <si>
+    <t>LightCyan</t>
+  </si>
+  <si>
+    <t>LightGreen</t>
+  </si>
+  <si>
+    <t>RoyalBlue</t>
+  </si>
+  <si>
+    <t>Sienna</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>SkyBlue</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Turquoise</t>
+  </si>
+  <si>
+    <t>Teal</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Violet</t>
+  </si>
+  <si>
+    <t>Crimson</t>
+  </si>
+  <si>
+    <t>SpringGreen</t>
   </si>
 </sst>
 </file>
@@ -690,7 +798,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,6 +807,8 @@
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -787,10 +897,10 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -810,10 +920,10 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
         <v>60</v>
-      </c>
-      <c r="G5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -833,10 +943,10 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -856,10 +966,10 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,10 +989,10 @@
         <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -902,7 +1012,7 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="G9" t="s">
         <v>61</v>
@@ -925,10 +1035,10 @@
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -948,10 +1058,10 @@
         <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="G11" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -971,10 +1081,10 @@
         <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -994,10 +1104,10 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1017,7 +1127,7 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="G14" t="s">
         <v>61</v>
@@ -1040,7 +1150,7 @@
         <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="G15" t="s">
         <v>61</v>
@@ -1063,10 +1173,10 @@
         <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1086,10 +1196,10 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" t="s">
         <v>60</v>
-      </c>
-      <c r="G17" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1109,10 +1219,10 @@
         <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="G18" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1132,10 +1242,10 @@
         <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="G19" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1155,10 +1265,10 @@
         <v>29</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1178,10 +1288,10 @@
         <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1201,10 +1311,10 @@
         <v>29</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="G22" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1224,10 +1334,10 @@
         <v>29</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="G23" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1247,10 +1357,10 @@
         <v>29</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>61</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1270,10 +1380,10 @@
         <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G25" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1296,7 +1406,7 @@
         <v>60</v>
       </c>
       <c r="G26" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1316,10 +1426,10 @@
         <v>29</v>
       </c>
       <c r="F27" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="G27" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1339,10 +1449,10 @@
         <v>29</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="G28" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1362,10 +1472,10 @@
         <v>29</v>
       </c>
       <c r="F29" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="G29" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1385,10 +1495,10 @@
         <v>29</v>
       </c>
       <c r="F30" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1408,10 +1518,10 @@
         <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="G31" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1431,10 +1541,10 @@
         <v>29</v>
       </c>
       <c r="F32" t="s">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="G32" t="s">
-        <v>61</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1454,7 +1564,7 @@
         <v>29</v>
       </c>
       <c r="F33" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="G33" t="s">
         <v>61</v>

</xml_diff>